<commit_message>
21-11-2023 ->11:01 Am Commit by Gvc
</commit_message>
<xml_diff>
--- a/src/test/resources/Automation.xlsx
+++ b/src/test/resources/Automation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="204">
   <si>
     <t>Schemes</t>
   </si>
@@ -748,46 +748,58 @@
     <t>KYC</t>
   </si>
   <si>
+    <t>First Details</t>
+  </si>
+  <si>
+    <t>Second Details</t>
+  </si>
+  <si>
     <t>Father Name</t>
   </si>
   <si>
     <t>Venkateswara Rao</t>
   </si>
   <si>
-    <t>Venkateswara Raoo</t>
+    <t>XYUG</t>
   </si>
   <si>
     <t>Spouse Name</t>
   </si>
   <si>
-    <t>Abcdefg</t>
-  </si>
-  <si>
     <t>jagadeesh</t>
   </si>
   <si>
+    <t>xyug</t>
+  </si>
+  <si>
     <t>Alternate Ph No</t>
   </si>
   <si>
-    <t>9848671412</t>
-  </si>
-  <si>
     <t>8331927870</t>
   </si>
   <si>
+    <t>9898989898</t>
+  </si>
+  <si>
     <t>Pan No</t>
   </si>
   <si>
-    <t>CTPPG2533D</t>
-  </si>
-  <si>
-    <t>ABCD1234K</t>
+    <t>ABCDE1123K</t>
+  </si>
+  <si>
+    <t>ABCDU1233K</t>
   </si>
   <si>
     <t>Aadhar No</t>
   </si>
   <si>
-    <t>436226303410</t>
+    <t>234567893411</t>
+  </si>
+  <si>
+    <t>456978941562</t>
+  </si>
+  <si>
+    <t>234567893410</t>
   </si>
   <si>
     <t>Nominee Details Updation</t>
@@ -841,55 +853,55 @@
     <t>Cousin</t>
   </si>
   <si>
+    <t>First Address</t>
+  </si>
+  <si>
     <t>Editing Details</t>
   </si>
   <si>
+    <t>Second Address</t>
+  </si>
+  <si>
     <t>Title</t>
   </si>
   <si>
-    <t>liveName</t>
-  </si>
-  <si>
-    <t>liveEdt</t>
-  </si>
-  <si>
-    <t>Staging</t>
-  </si>
-  <si>
-    <t>stgEdt</t>
-  </si>
-  <si>
-    <t>livePrakash Nagar</t>
-  </si>
-  <si>
-    <t>liveBegumpetEdt</t>
-  </si>
-  <si>
-    <t>StgPrakash Nagar</t>
-  </si>
-  <si>
-    <t>StgBegumpet</t>
-  </si>
-  <si>
-    <t>liveHyderabad</t>
-  </si>
-  <si>
-    <t>liveSecunderabad</t>
-  </si>
-  <si>
-    <t>StgHyderabad</t>
-  </si>
-  <si>
-    <t>StgSecunderabad</t>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Home1</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>522</t>
+  </si>
+  <si>
+    <t>118 CNR</t>
+  </si>
+  <si>
+    <t>Hyd</t>
+  </si>
+  <si>
+    <t>Guntur</t>
   </si>
   <si>
     <t>Telangana</t>
   </si>
   <si>
-    <t>528008</t>
-  </si>
-  <si>
-    <t>532650</t>
+    <t>Ap</t>
+  </si>
+  <si>
+    <t>Tel</t>
+  </si>
+  <si>
+    <t>500015</t>
+  </si>
+  <si>
+    <t>500010</t>
   </si>
   <si>
     <t>Bank Accounts</t>
@@ -910,49 +922,49 @@
     <t>Name On Account</t>
   </si>
   <si>
-    <t>Vicky</t>
+    <t>Pavanikaka</t>
+  </si>
+  <si>
+    <t>Pavanik</t>
   </si>
   <si>
     <t>Account No</t>
   </si>
   <si>
-    <t>1513059123</t>
-  </si>
-  <si>
-    <t>1513059234</t>
+    <t>00000000118</t>
+  </si>
+  <si>
+    <t>23400000000118</t>
   </si>
   <si>
     <t>1513059876</t>
   </si>
   <si>
-    <t>151305917</t>
-  </si>
-  <si>
-    <t>32809171253</t>
-  </si>
-  <si>
     <t>Bank Name</t>
   </si>
   <si>
-    <t>Kotak</t>
-  </si>
-  <si>
-    <t>Sbi</t>
+    <t>Axis Bank</t>
+  </si>
+  <si>
+    <t>Union Bank</t>
   </si>
   <si>
     <t>Branch</t>
   </si>
   <si>
-    <t>Nellore</t>
+    <t>Alwal</t>
+  </si>
+  <si>
+    <t>Manikonda</t>
   </si>
   <si>
     <t>Ifsc code</t>
   </si>
   <si>
-    <t>KKBK007805</t>
-  </si>
-  <si>
-    <t>SBIN0007457</t>
+    <t>AXIS1237456</t>
+  </si>
+  <si>
+    <t>UNIB1234569</t>
   </si>
   <si>
     <t>NEGATIVE DATA</t>
@@ -1031,7 +1043,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1062,6 +1074,12 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -1562,128 +1580,128 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
@@ -1691,17 +1709,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2040,8 +2058,8 @@
     <col min="12" max="12" width="18.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="1" spans="7:7">
-      <c r="G1" s="13" t="s">
+    <row r="1" s="11" customFormat="1" spans="7:7">
+      <c r="G1" s="12" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2049,25 +2067,25 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="J2" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2075,25 +2093,25 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="14" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2101,25 +2119,25 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>3</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>4</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2127,25 +2145,25 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>10</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2153,25 +2171,25 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>13</v>
       </c>
       <c r="J7" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2179,25 +2197,25 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>7</v>
       </c>
       <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="14" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2205,25 +2223,25 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="14" t="s">
         <v>13</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="14" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2231,25 +2249,25 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2257,25 +2275,25 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>16</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="15" t="s">
+      <c r="H12" s="14" t="s">
         <v>17</v>
       </c>
       <c r="J12" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2283,25 +2301,25 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="14" t="s">
         <v>7</v>
       </c>
       <c r="J13" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="14" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2309,25 +2327,25 @@
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>15</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="14" t="s">
         <v>16</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>17</v>
       </c>
       <c r="J14" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2335,30 +2353,30 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="14" t="s">
         <v>10</v>
       </c>
       <c r="J15" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="10:10">
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2366,31 +2384,31 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="14" t="s">
         <v>21</v>
       </c>
       <c r="G17" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="14" t="s">
         <v>22</v>
       </c>
       <c r="J17" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="14" t="s">
         <v>24</v>
       </c>
       <c r="L17" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="15" t="s">
+      <c r="M17" s="14" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2398,31 +2416,31 @@
       <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="14" t="s">
         <v>7</v>
       </c>
       <c r="J18" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="14" t="s">
         <v>26</v>
       </c>
       <c r="L18" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="15" t="s">
+      <c r="M18" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2430,31 +2448,31 @@
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>21</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="14" t="s">
         <v>22</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="14" t="s">
         <v>28</v>
       </c>
       <c r="L19" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="15" t="s">
+      <c r="M19" s="14" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2462,31 +2480,31 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="14" t="s">
         <v>10</v>
       </c>
       <c r="J20" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="14" t="s">
         <v>30</v>
       </c>
       <c r="L20" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="15" t="s">
+      <c r="M20" s="14" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2494,13 +2512,13 @@
       <c r="J21" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="15" t="s">
+      <c r="K21" s="14" t="s">
         <v>32</v>
       </c>
       <c r="L21" t="s">
         <v>23</v>
       </c>
-      <c r="M21" s="15" t="s">
+      <c r="M21" s="14" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2508,31 +2526,31 @@
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>35</v>
       </c>
       <c r="G22" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="14" t="s">
         <v>36</v>
       </c>
       <c r="J22" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="15" t="s">
+      <c r="K22" s="14" t="s">
         <v>37</v>
       </c>
       <c r="L22" t="s">
         <v>23</v>
       </c>
-      <c r="M22" s="15" t="s">
+      <c r="M22" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2540,31 +2558,31 @@
       <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G23" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="14" t="s">
         <v>7</v>
       </c>
       <c r="J23" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="14" t="s">
         <v>39</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
       </c>
-      <c r="M23" s="15" t="s">
+      <c r="M23" s="14" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2572,31 +2590,31 @@
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="14" t="s">
         <v>35</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="14" t="s">
         <v>36</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="15" t="s">
+      <c r="K24" s="14" t="s">
         <v>41</v>
       </c>
       <c r="L24" t="s">
         <v>23</v>
       </c>
-      <c r="M24" s="15" t="s">
+      <c r="M24" s="14" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2604,31 +2622,31 @@
       <c r="A25" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="14" t="s">
         <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="14" t="s">
         <v>10</v>
       </c>
       <c r="J25" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="K25" s="14" t="s">
         <v>43</v>
       </c>
       <c r="L25" t="s">
         <v>23</v>
       </c>
-      <c r="M25" s="15" t="s">
+      <c r="M25" s="14" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2651,32 +2669,32 @@
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2701,257 +2719,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="10" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="10" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="10" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="10" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="10" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="10" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="10" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="10" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="10" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2964,13 +2982,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24.7777777777778" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
@@ -2978,6 +2996,7 @@
     <col min="6" max="6" width="15.1111111111111" customWidth="1"/>
     <col min="7" max="7" width="23.5555555555556" customWidth="1"/>
     <col min="8" max="8" width="14.8888888888889" customWidth="1"/>
+    <col min="9" max="9" width="13.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3014,76 +3033,97 @@
       <c r="A4" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="G6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>115</v>
+      </c>
+      <c r="H7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>118</v>
+      </c>
+      <c r="H8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="G9" s="15" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="B9" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>124</v>
+      </c>
+      <c r="H10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>125</v>
+        <v>128</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -3091,319 +3131,361 @@
         <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="G14" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>129</v>
+        <v>132</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="G16" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G17" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="G18" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="G19" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>139</v>
+        <v>142</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" t="s">
+        <v>153</v>
+      </c>
+      <c r="G24" t="s">
+        <v>151</v>
+      </c>
+      <c r="H24" t="s">
+        <v>152</v>
+      </c>
+      <c r="I24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" t="s">
+        <v>156</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="I25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" t="s">
+        <v>158</v>
+      </c>
+      <c r="I26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G27" t="s">
+        <v>159</v>
+      </c>
+      <c r="H27" t="s">
+        <v>160</v>
+      </c>
+      <c r="I27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>144</v>
-      </c>
-      <c r="B24" t="s">
-        <v>145</v>
-      </c>
-      <c r="C24" t="s">
-        <v>146</v>
-      </c>
-      <c r="G24" t="s">
-        <v>147</v>
-      </c>
-      <c r="H24" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" t="s">
-        <v>149</v>
-      </c>
-      <c r="C25" t="s">
-        <v>150</v>
-      </c>
-      <c r="G25" t="s">
-        <v>151</v>
-      </c>
-      <c r="H25" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
-        <v>132</v>
-      </c>
-      <c r="B26" t="s">
-        <v>153</v>
-      </c>
-      <c r="C26" t="s">
-        <v>154</v>
-      </c>
-      <c r="G26" t="s">
-        <v>155</v>
-      </c>
-      <c r="H26" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B27" t="s">
-        <v>157</v>
-      </c>
-      <c r="C27" t="s">
-        <v>135</v>
-      </c>
-      <c r="G27" t="s">
-        <v>157</v>
-      </c>
-      <c r="H27" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>159</v>
+      <c r="B28" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>161</v>
+        <v>148</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>165</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>167</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
-      </c>
-      <c r="D31" s="5"/>
+        <v>168</v>
+      </c>
+      <c r="D31" s="6"/>
       <c r="G31" t="s">
-        <v>103</v>
+        <v>167</v>
       </c>
       <c r="H31" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>164</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>166</v>
+        <v>169</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>171</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>167</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>169</v>
+        <v>172</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B33" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C33" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G33" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H33" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B34" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C34" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G34" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H34" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B35" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C35" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="G35" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="H35" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="7" t="s">
-        <v>178</v>
+      <c r="A37" s="8" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B38" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C38" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D38" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="E38" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F38" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="G38" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:1">
@@ -3413,105 +3495,105 @@
       <c r="A41" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>187</v>
+      <c r="B41" s="14" t="s">
+        <v>191</v>
       </c>
       <c r="C41" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="F41" s="15" t="s">
-        <v>187</v>
+      <c r="D41" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>105</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>189</v>
+      <c r="B42" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>190</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>192</v>
+        <v>194</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>196</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>115</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>196</v>
+        <v>117</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>118</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>197</v>
+        <v>120</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>121</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>198</v>
+        <v>123</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>124</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>199</v>
+        <v>126</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
25-11-2023 Updated Code Committed by GVC
</commit_message>
<xml_diff>
--- a/src/test/resources/Automation.xlsx
+++ b/src/test/resources/Automation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="227">
   <si>
     <t>Schemes</t>
   </si>
@@ -1031,6 +1031,115 @@
   </si>
   <si>
     <t>12345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nominee Details </t>
+  </si>
+  <si>
+    <t>Invalid Details</t>
+  </si>
+  <si>
+    <t>@#$%^</t>
+  </si>
+  <si>
+    <t>PhoneNo</t>
+  </si>
+  <si>
+    <t>630@@@1234568</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Alwal</t>
+    </r>
+  </si>
+  <si>
+    <t>@123l</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Hyd</t>
+    </r>
+  </si>
+  <si>
+    <t>Hyd@#</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Telangana</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Afghanistan</t>
+    </r>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>5000151234</t>
+  </si>
+  <si>
+    <t>500016786</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF1F1F1F"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Brother</t>
+    </r>
+  </si>
+  <si>
+    <t>Home @123</t>
+  </si>
+  <si>
+    <t>Hyd#0000</t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>000000000000</t>
+  </si>
+  <si>
+    <t>123#@</t>
+  </si>
+  <si>
+    <t>FullName as per Bank</t>
+  </si>
+  <si>
+    <t>Account Number</t>
+  </si>
+  <si>
+    <t>1234567890990</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1152,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1104,6 +1213,24 @@
       <sz val="9.75"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Consolas"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1580,128 +1707,128 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
@@ -1713,6 +1840,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2058,8 +2191,8 @@
     <col min="12" max="12" width="18.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" spans="7:7">
-      <c r="G1" s="12" t="s">
+    <row r="1" s="15" customFormat="1" spans="7:7">
+      <c r="G1" s="16" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2067,25 +2200,25 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="J2" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2093,25 +2226,25 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2119,25 +2252,25 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="18" t="s">
         <v>4</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2145,25 +2278,25 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2171,25 +2304,25 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="18" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J7" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2197,25 +2330,25 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2223,25 +2356,25 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="18" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2249,25 +2382,25 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2275,25 +2408,25 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="18" t="s">
         <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="18" t="s">
         <v>16</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="18" t="s">
         <v>17</v>
       </c>
       <c r="J12" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="K12" s="18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2301,25 +2434,25 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J13" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K13" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2327,25 +2460,25 @@
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="18" t="s">
         <v>15</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="18" t="s">
         <v>16</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="18" t="s">
         <v>17</v>
       </c>
       <c r="J14" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2353,30 +2486,30 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J15" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="K15" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="10:10">
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2384,31 +2517,31 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="18" t="s">
         <v>21</v>
       </c>
       <c r="G17" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="18" t="s">
         <v>22</v>
       </c>
       <c r="J17" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="18" t="s">
         <v>24</v>
       </c>
       <c r="L17" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="14" t="s">
+      <c r="M17" s="18" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2416,31 +2549,31 @@
       <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J18" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="K18" s="18" t="s">
         <v>26</v>
       </c>
       <c r="L18" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="M18" s="18" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2448,31 +2581,31 @@
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="18" t="s">
         <v>21</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="18" t="s">
         <v>22</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="K19" s="18" t="s">
         <v>28</v>
       </c>
       <c r="L19" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="14" t="s">
+      <c r="M19" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2480,31 +2613,31 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J20" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="18" t="s">
         <v>30</v>
       </c>
       <c r="L20" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2512,13 +2645,13 @@
       <c r="J21" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="K21" s="18" t="s">
         <v>32</v>
       </c>
       <c r="L21" t="s">
         <v>23</v>
       </c>
-      <c r="M21" s="14" t="s">
+      <c r="M21" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2526,31 +2659,31 @@
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="18" t="s">
         <v>35</v>
       </c>
       <c r="G22" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="18" t="s">
         <v>36</v>
       </c>
       <c r="J22" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="18" t="s">
         <v>37</v>
       </c>
       <c r="L22" t="s">
         <v>23</v>
       </c>
-      <c r="M22" s="14" t="s">
+      <c r="M22" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2558,31 +2691,31 @@
       <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G23" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J23" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="14" t="s">
+      <c r="K23" s="18" t="s">
         <v>39</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
       </c>
-      <c r="M23" s="14" t="s">
+      <c r="M23" s="18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2590,31 +2723,31 @@
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="18" t="s">
         <v>35</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="18" t="s">
         <v>36</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="18" t="s">
         <v>41</v>
       </c>
       <c r="L24" t="s">
         <v>23</v>
       </c>
-      <c r="M24" s="14" t="s">
+      <c r="M24" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2622,31 +2755,31 @@
       <c r="A25" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J25" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="14" t="s">
+      <c r="K25" s="18" t="s">
         <v>43</v>
       </c>
       <c r="L25" t="s">
         <v>23</v>
       </c>
-      <c r="M25" s="14" t="s">
+      <c r="M25" s="18" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2669,32 +2802,32 @@
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2719,257 +2852,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="14" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="14" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="14" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="14" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="14" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="14" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="14" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="14" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="14" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="14" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="14" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="14" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="14" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="14" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="14" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="14" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="14" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="14" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="14" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="14" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="14" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="14" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="14" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="14" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="14" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="14" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2982,10 +3115,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -3033,10 +3166,10 @@
       <c r="A4" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="18" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3083,13 +3216,13 @@
       <c r="A9" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="18" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3111,13 +3244,13 @@
       <c r="A11" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="18" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3141,10 +3274,10 @@
       <c r="A15" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="18" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3196,10 +3329,10 @@
       <c r="A20" t="s">
         <v>142</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="18" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3264,19 +3397,19 @@
       <c r="A25" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="18" t="s">
         <v>155</v>
       </c>
       <c r="D25" t="s">
         <v>156</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="18" t="s">
         <v>155</v>
       </c>
       <c r="I25" t="s">
@@ -3333,22 +3466,22 @@
       <c r="A28" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="18" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3388,19 +3521,19 @@
       <c r="A32" t="s">
         <v>169</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="18" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3495,19 +3628,19 @@
       <c r="A41" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="18" t="s">
         <v>191</v>
       </c>
       <c r="C41" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41">
+        <v>12345</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="E41" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="18" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3535,19 +3668,19 @@
       <c r="A43" t="s">
         <v>194</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="F43" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="G43" s="17" t="s">
+      <c r="G43" s="21" t="s">
         <v>197</v>
       </c>
     </row>
@@ -3568,7 +3701,7 @@
       <c r="A48" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="18" t="s">
         <v>200</v>
       </c>
     </row>
@@ -3576,7 +3709,7 @@
       <c r="A49" t="s">
         <v>120</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="18" t="s">
         <v>201</v>
       </c>
     </row>
@@ -3584,7 +3717,7 @@
       <c r="A50" t="s">
         <v>123</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="18" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3592,8 +3725,192 @@
       <c r="A51" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="18" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4">
+      <c r="D54" s="10"/>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>207</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C57" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>138</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>215</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D64" s="10"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>150</v>
+      </c>
+      <c r="B66" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" t="s">
+        <v>157</v>
+      </c>
+      <c r="C67" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>221</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" t="s">
+        <v>177</v>
+      </c>
+      <c r="C70" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>225</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -3605,6 +3922,7 @@
     <hyperlink ref="D42" r:id="rId4" display="pavanikaka@gmail.com"/>
     <hyperlink ref="E42" r:id="rId4" display="pavanikaka@gmail.com"/>
     <hyperlink ref="G42" r:id="rId4" display="pavanikaka@gmail.com"/>
+    <hyperlink ref="C58" r:id="rId5" display="Hyd@#"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
28-11-2023 After Testing Changes Pushed by Gvc
</commit_message>
<xml_diff>
--- a/src/test/resources/Automation.xlsx
+++ b/src/test/resources/Automation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="229">
   <si>
     <t>Schemes</t>
   </si>
@@ -997,6 +997,9 @@
     <t>12345</t>
   </si>
   <si>
+    <t>Gvc</t>
+  </si>
+  <si>
     <t>123@gmail.com</t>
   </si>
   <si>
@@ -1010,6 +1013,9 @@
   </si>
   <si>
     <t>7546613511</t>
+  </si>
+  <si>
+    <t>630</t>
   </si>
   <si>
     <t>6309631698</t>
@@ -1828,7 +1834,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
@@ -1840,7 +1846,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2191,8 +2196,8 @@
     <col min="12" max="12" width="18.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="1" spans="7:7">
-      <c r="G1" s="16" t="s">
+    <row r="1" s="14" customFormat="1" spans="7:7">
+      <c r="G1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2200,25 +2205,25 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>4</v>
       </c>
       <c r="J2" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2226,25 +2231,25 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2252,25 +2257,25 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>3</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>4</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2278,25 +2283,25 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2304,25 +2309,25 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>13</v>
       </c>
       <c r="J7" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2330,25 +2335,25 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2356,25 +2361,25 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>13</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2382,25 +2387,25 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2408,25 +2413,25 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="J12" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2434,25 +2439,25 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J13" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2460,25 +2465,25 @@
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="17" t="s">
         <v>16</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="17" t="s">
         <v>17</v>
       </c>
       <c r="J14" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2486,30 +2491,30 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J15" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="K15" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="10:10">
-      <c r="J16" s="17" t="s">
+      <c r="J16" s="16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2517,31 +2522,31 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>21</v>
       </c>
       <c r="G17" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>22</v>
       </c>
       <c r="J17" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="18" t="s">
+      <c r="K17" s="17" t="s">
         <v>24</v>
       </c>
       <c r="L17" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="18" t="s">
+      <c r="M17" s="17" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2549,31 +2554,31 @@
       <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J18" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="18" t="s">
+      <c r="K18" s="17" t="s">
         <v>26</v>
       </c>
       <c r="L18" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="18" t="s">
+      <c r="M18" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2581,31 +2586,31 @@
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="17" t="s">
         <v>21</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="17" t="s">
         <v>22</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="17" t="s">
         <v>28</v>
       </c>
       <c r="L19" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="18" t="s">
+      <c r="M19" s="17" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2613,31 +2618,31 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J20" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="17" t="s">
         <v>30</v>
       </c>
       <c r="L20" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="18" t="s">
+      <c r="M20" s="17" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2645,13 +2650,13 @@
       <c r="J21" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="18" t="s">
+      <c r="K21" s="17" t="s">
         <v>32</v>
       </c>
       <c r="L21" t="s">
         <v>23</v>
       </c>
-      <c r="M21" s="18" t="s">
+      <c r="M21" s="17" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2659,31 +2664,31 @@
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="17" t="s">
         <v>35</v>
       </c>
       <c r="G22" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="17" t="s">
         <v>36</v>
       </c>
       <c r="J22" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="18" t="s">
+      <c r="K22" s="17" t="s">
         <v>37</v>
       </c>
       <c r="L22" t="s">
         <v>23</v>
       </c>
-      <c r="M22" s="18" t="s">
+      <c r="M22" s="17" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2691,31 +2696,31 @@
       <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G23" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H23" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J23" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="18" t="s">
+      <c r="K23" s="17" t="s">
         <v>39</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
       </c>
-      <c r="M23" s="18" t="s">
+      <c r="M23" s="17" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2723,31 +2728,31 @@
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="17" t="s">
         <v>35</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="17" t="s">
         <v>36</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="18" t="s">
+      <c r="K24" s="17" t="s">
         <v>41</v>
       </c>
       <c r="L24" t="s">
         <v>23</v>
       </c>
-      <c r="M24" s="18" t="s">
+      <c r="M24" s="17" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2755,31 +2760,31 @@
       <c r="A25" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J25" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="18" t="s">
+      <c r="K25" s="17" t="s">
         <v>43</v>
       </c>
       <c r="L25" t="s">
         <v>23</v>
       </c>
-      <c r="M25" s="18" t="s">
+      <c r="M25" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2802,32 +2807,32 @@
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2852,257 +2857,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="13" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="13" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="13" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="13" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="13" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="13" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="13" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3117,8 +3122,8 @@
   <sheetPr/>
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -3166,10 +3171,10 @@
       <c r="A4" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3216,13 +3221,13 @@
       <c r="A9" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3244,13 +3249,13 @@
       <c r="A11" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3274,10 +3279,10 @@
       <c r="A15" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="17" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3329,10 +3334,10 @@
       <c r="A20" t="s">
         <v>142</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="17" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3397,19 +3402,19 @@
       <c r="A25" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="17" t="s">
         <v>155</v>
       </c>
       <c r="D25" t="s">
         <v>156</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="17" t="s">
         <v>155</v>
       </c>
       <c r="I25" t="s">
@@ -3466,22 +3471,22 @@
       <c r="A28" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="G28" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="17" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3521,19 +3526,19 @@
       <c r="A32" t="s">
         <v>169</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="17" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3628,7 +3633,7 @@
       <c r="A41" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="17" t="s">
         <v>191</v>
       </c>
       <c r="C41" t="s">
@@ -3637,11 +3642,11 @@
       <c r="D41">
         <v>12345</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="F41" s="18" t="s">
-        <v>191</v>
+      <c r="F41" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -3649,44 +3654,44 @@
         <v>105</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>194</v>
-      </c>
-      <c r="B43" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="C43" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="D43" s="18" t="s">
+      <c r="B43" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="C43" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D43" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="G43" s="21" t="s">
-        <v>197</v>
+      <c r="F43" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -3694,47 +3699,47 @@
         <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="18" t="s">
-        <v>200</v>
+      <c r="B48" s="17" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>120</v>
       </c>
-      <c r="B49" s="18" t="s">
-        <v>201</v>
+      <c r="B49" s="17" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>123</v>
       </c>
-      <c r="B50" s="18" t="s">
-        <v>202</v>
+      <c r="B50" s="17" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="18" t="s">
-        <v>203</v>
+      <c r="B51" s="17" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="4:4">
@@ -3748,18 +3753,18 @@
         <v>104</v>
       </c>
       <c r="C55" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>207</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -3767,10 +3772,10 @@
         <v>134</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C57" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -3778,54 +3783,54 @@
         <v>136</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>213</v>
+      <c r="B59" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>140</v>
       </c>
-      <c r="B60" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>214</v>
+      <c r="B60" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>215</v>
-      </c>
-      <c r="B61" s="19" t="s">
-        <v>216</v>
-      </c>
-      <c r="C61" s="18" t="s">
         <v>217</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>144</v>
       </c>
-      <c r="B62" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>218</v>
+      <c r="B62" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -3833,7 +3838,7 @@
         <v>134</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D64" s="10"/>
     </row>
@@ -3844,8 +3849,8 @@
       <c r="B66" t="s">
         <v>151</v>
       </c>
-      <c r="C66" s="11" t="s">
-        <v>219</v>
+      <c r="C66" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -3856,29 +3861,29 @@
         <v>157</v>
       </c>
       <c r="C67" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>138</v>
       </c>
-      <c r="B68" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>213</v>
+      <c r="B68" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>221</v>
-      </c>
-      <c r="B69" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B69" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="C69" s="18" t="s">
-        <v>222</v>
+      <c r="C69" s="17" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -3889,7 +3894,7 @@
         <v>177</v>
       </c>
       <c r="C70" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="72" spans="1:1">
@@ -3899,7 +3904,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B74" t="s">
         <v>167</v>
@@ -3907,10 +3912,10 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>225</v>
-      </c>
-      <c r="B75" s="18" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
02-12-2023 Recent Changes commited
</commit_message>
<xml_diff>
--- a/src/test/resources/Automation.xlsx
+++ b/src/test/resources/Automation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="241">
   <si>
     <t>Schemes</t>
   </si>
@@ -1000,12 +1000,18 @@
     <t>Gvc</t>
   </si>
   <si>
+    <t>##@$!</t>
+  </si>
+  <si>
     <t>123@gmail.com</t>
   </si>
   <si>
     <t>pavanikaka@gmail.com</t>
   </si>
   <si>
+    <t>148@#$</t>
+  </si>
+  <si>
     <t>MobileNo</t>
   </si>
   <si>
@@ -1021,37 +1027,58 @@
     <t>6309631698</t>
   </si>
   <si>
+    <t>986</t>
+  </si>
+  <si>
     <t>KYC DATA</t>
   </si>
   <si>
     <t>P123</t>
   </si>
   <si>
+    <t>@#$%^</t>
+  </si>
+  <si>
     <t>1244</t>
   </si>
   <si>
     <t>0000</t>
   </si>
   <si>
+    <t>#$%^&amp;$%^&amp;$%</t>
+  </si>
+  <si>
     <t>00000</t>
   </si>
   <si>
+    <t>#$%^&amp;$%</t>
+  </si>
+  <si>
     <t>12345678</t>
   </si>
   <si>
+    <t>!@#$%^&amp;*()!@</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nominee Details </t>
   </si>
   <si>
     <t>Invalid Details</t>
   </si>
   <si>
-    <t>@#$%^</t>
+    <t>All Special Chars</t>
+  </si>
+  <si>
+    <t>!@#$%^&amp;!@#</t>
   </si>
   <si>
     <t>PhoneNo</t>
   </si>
   <si>
     <t>630@@@1234568</t>
+  </si>
+  <si>
+    <t>@#$%^&amp;*(</t>
   </si>
   <si>
     <r>
@@ -1068,6 +1095,9 @@
     <t>@123l</t>
   </si>
   <si>
+    <t>!@#$%^&amp;*(6</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="9"/>
@@ -1080,6 +1110,9 @@
   </si>
   <si>
     <t>Hyd@#</t>
+  </si>
+  <si>
+    <t>*&amp;^%$#@!</t>
   </si>
   <si>
     <r>
@@ -1111,6 +1144,9 @@
   </si>
   <si>
     <t>500016786</t>
+  </si>
+  <si>
+    <t>@#$%^&amp;</t>
   </si>
   <si>
     <r>
@@ -1834,7 +1870,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
@@ -1844,6 +1880,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2196,8 +2233,8 @@
     <col min="12" max="12" width="18.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="1" spans="7:7">
-      <c r="G1" s="15" t="s">
+    <row r="1" s="15" customFormat="1" spans="7:7">
+      <c r="G1" s="16" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2205,25 +2242,25 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="18" t="s">
         <v>4</v>
       </c>
       <c r="J2" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2231,25 +2268,25 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2257,25 +2294,25 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="18" t="s">
         <v>4</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2283,25 +2320,25 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2309,25 +2346,25 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="18" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J7" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="17" t="s">
+      <c r="K7" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2335,25 +2372,25 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2361,25 +2398,25 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="18" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="18" t="s">
         <v>13</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="K9" s="18" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2387,25 +2424,25 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="17" t="s">
+      <c r="K10" s="18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2413,25 +2450,25 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="18" t="s">
         <v>16</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="18" t="s">
         <v>17</v>
       </c>
       <c r="J12" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="K12" s="18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2439,25 +2476,25 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J13" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="K13" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2465,25 +2502,25 @@
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="18" t="s">
         <v>15</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="18" t="s">
         <v>16</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="18" t="s">
         <v>17</v>
       </c>
       <c r="J14" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="K14" s="18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2491,30 +2528,30 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J15" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="K15" s="18" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="10:10">
-      <c r="J16" s="16" t="s">
+      <c r="J16" s="17" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2522,31 +2559,31 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="18" t="s">
         <v>21</v>
       </c>
       <c r="G17" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="18" t="s">
         <v>22</v>
       </c>
       <c r="J17" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="17" t="s">
+      <c r="K17" s="18" t="s">
         <v>24</v>
       </c>
       <c r="L17" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="17" t="s">
+      <c r="M17" s="18" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2554,31 +2591,31 @@
       <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J18" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="17" t="s">
+      <c r="K18" s="18" t="s">
         <v>26</v>
       </c>
       <c r="L18" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="17" t="s">
+      <c r="M18" s="18" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2586,31 +2623,31 @@
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="18" t="s">
         <v>21</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="18" t="s">
         <v>22</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="17" t="s">
+      <c r="K19" s="18" t="s">
         <v>28</v>
       </c>
       <c r="L19" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="17" t="s">
+      <c r="M19" s="18" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2618,31 +2655,31 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J20" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="17" t="s">
+      <c r="K20" s="18" t="s">
         <v>30</v>
       </c>
       <c r="L20" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="17" t="s">
+      <c r="M20" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2650,13 +2687,13 @@
       <c r="J21" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="17" t="s">
+      <c r="K21" s="18" t="s">
         <v>32</v>
       </c>
       <c r="L21" t="s">
         <v>23</v>
       </c>
-      <c r="M21" s="17" t="s">
+      <c r="M21" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2664,31 +2701,31 @@
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="18" t="s">
         <v>35</v>
       </c>
       <c r="G22" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="18" t="s">
         <v>36</v>
       </c>
       <c r="J22" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="17" t="s">
+      <c r="K22" s="18" t="s">
         <v>37</v>
       </c>
       <c r="L22" t="s">
         <v>23</v>
       </c>
-      <c r="M22" s="17" t="s">
+      <c r="M22" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2696,31 +2733,31 @@
       <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="18" t="s">
         <v>7</v>
       </c>
       <c r="G23" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="18" t="s">
         <v>7</v>
       </c>
       <c r="J23" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="17" t="s">
+      <c r="K23" s="18" t="s">
         <v>39</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
       </c>
-      <c r="M23" s="17" t="s">
+      <c r="M23" s="18" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2728,31 +2765,31 @@
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="18" t="s">
         <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="18" t="s">
         <v>35</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H24" s="18" t="s">
         <v>36</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="17" t="s">
+      <c r="K24" s="18" t="s">
         <v>41</v>
       </c>
       <c r="L24" t="s">
         <v>23</v>
       </c>
-      <c r="M24" s="17" t="s">
+      <c r="M24" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2760,31 +2797,31 @@
       <c r="A25" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="18" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="18" t="s">
         <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="18" t="s">
         <v>10</v>
       </c>
       <c r="J25" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="17" t="s">
+      <c r="K25" s="18" t="s">
         <v>43</v>
       </c>
       <c r="L25" t="s">
         <v>23</v>
       </c>
-      <c r="M25" s="17" t="s">
+      <c r="M25" s="18" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2807,32 +2844,32 @@
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2857,257 +2894,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="14" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="14" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="14" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="14" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="14" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="14" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="14" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="14" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="14" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="14" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="14" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="14" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="14" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="14" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="14" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="14" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="14" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="14" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="14" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="14" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="14" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="14" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="14" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="14" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="14" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="14" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3122,8 +3159,8 @@
   <sheetPr/>
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -3133,7 +3170,7 @@
     <col min="3" max="5" width="22.4444444444444" customWidth="1"/>
     <col min="6" max="6" width="15.1111111111111" customWidth="1"/>
     <col min="7" max="7" width="23.5555555555556" customWidth="1"/>
-    <col min="8" max="8" width="14.8888888888889" customWidth="1"/>
+    <col min="8" max="8" width="20.4444444444444" customWidth="1"/>
     <col min="9" max="9" width="13.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3171,10 +3208,10 @@
       <c r="A4" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="18" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3221,13 +3258,13 @@
       <c r="A9" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="18" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3249,13 +3286,13 @@
       <c r="A11" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="18" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3279,10 +3316,10 @@
       <c r="A15" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="18" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3334,10 +3371,10 @@
       <c r="A20" t="s">
         <v>142</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="18" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3402,19 +3439,19 @@
       <c r="A25" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="18" t="s">
         <v>155</v>
       </c>
       <c r="D25" t="s">
         <v>156</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="18" t="s">
         <v>155</v>
       </c>
       <c r="I25" t="s">
@@ -3471,22 +3508,22 @@
       <c r="A28" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D28" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="H28" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="I28" s="17" t="s">
+      <c r="I28" s="18" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3526,19 +3563,19 @@
       <c r="A32" t="s">
         <v>169</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="G32" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="18" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3629,11 +3666,11 @@
     <row r="40" spans="1:1">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="18" t="s">
         <v>191</v>
       </c>
       <c r="C41" t="s">
@@ -3642,110 +3679,137 @@
       <c r="D41">
         <v>12345</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="18" t="s">
         <v>191</v>
       </c>
       <c r="F41" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>105</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>195</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>195</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="D43" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="B43" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="G43" s="20" t="s">
+      <c r="C43" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="D43" s="18" t="s">
         <v>199</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>204</v>
+      </c>
+      <c r="C47" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="17" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="B48" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>120</v>
       </c>
-      <c r="B49" s="17" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="B49" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>123</v>
       </c>
-      <c r="B50" s="17" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="B50" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="C50" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="17" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="B51" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="C51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>207</v>
+        <v>214</v>
+      </c>
+      <c r="D53" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="54" spans="4:4">
-      <c r="D54" s="10"/>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" s="11"/>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>102</v>
       </c>
@@ -3753,84 +3817,108 @@
         <v>104</v>
       </c>
       <c r="C55" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>205</v>
+      </c>
+      <c r="D55" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>209</v>
-      </c>
-      <c r="B56" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>217</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="D56" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>134</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C57" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>221</v>
+      </c>
+      <c r="D57" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>136</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>224</v>
+      </c>
+      <c r="D58" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="B59" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>140</v>
       </c>
-      <c r="B60" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="B60" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>217</v>
-      </c>
-      <c r="B61" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>228</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="D61" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>144</v>
       </c>
-      <c r="B62" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>220</v>
+      <c r="B62" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -3838,9 +3926,9 @@
         <v>134</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D64" s="10"/>
+        <v>214</v>
+      </c>
+      <c r="D64" s="11"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
@@ -3850,7 +3938,7 @@
         <v>151</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
     </row>
     <row r="67" spans="1:3">
@@ -3861,29 +3949,29 @@
         <v>157</v>
       </c>
       <c r="C67" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>138</v>
       </c>
-      <c r="B68" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>215</v>
+      <c r="B68" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>223</v>
-      </c>
-      <c r="B69" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="B69" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="C69" s="17" t="s">
-        <v>224</v>
+      <c r="C69" s="18" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -3894,7 +3982,7 @@
         <v>177</v>
       </c>
       <c r="C70" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
     </row>
     <row r="72" spans="1:1">
@@ -3904,7 +3992,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="B74" t="s">
         <v>167</v>
@@ -3912,10 +4000,10 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>227</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>228</v>
+        <v>239</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -3928,6 +4016,7 @@
     <hyperlink ref="E42" r:id="rId4" display="pavanikaka@gmail.com"/>
     <hyperlink ref="G42" r:id="rId4" display="pavanikaka@gmail.com"/>
     <hyperlink ref="C58" r:id="rId5" display="Hyd@#"/>
+    <hyperlink ref="H42" r:id="rId6" display="148@#$"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
commited by GVC on 4-12-2023
</commit_message>
<xml_diff>
--- a/src/test/resources/Automation.xlsx
+++ b/src/test/resources/Automation.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="255">
   <si>
     <t>Schemes</t>
   </si>
@@ -1028,6 +1028,9 @@
   </si>
   <si>
     <t>986</t>
+  </si>
+  <si>
+    <t>987</t>
   </si>
   <si>
     <t>KYC DATA</t>
@@ -1909,7 +1912,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
@@ -1919,7 +1922,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2272,8 +2274,8 @@
     <col min="12" max="12" width="18.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="1" spans="7:7">
-      <c r="G1" s="16" t="s">
+    <row r="1" s="14" customFormat="1" spans="7:7">
+      <c r="G1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2281,25 +2283,25 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>4</v>
       </c>
       <c r="J2" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2307,25 +2309,25 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2333,25 +2335,25 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>3</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>4</v>
       </c>
       <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2359,25 +2361,25 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2385,25 +2387,25 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="17" t="s">
         <v>13</v>
       </c>
       <c r="J7" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2411,25 +2413,25 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J8" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2437,25 +2439,25 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>12</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>13</v>
       </c>
       <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2463,25 +2465,25 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J10" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2489,25 +2491,25 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>16</v>
       </c>
       <c r="G12" t="s">
         <v>1</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>17</v>
       </c>
       <c r="J12" t="s">
         <v>1</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2515,25 +2517,25 @@
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J13" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2541,25 +2543,25 @@
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="17" t="s">
         <v>16</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="17" t="s">
         <v>17</v>
       </c>
       <c r="J14" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="17" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2567,30 +2569,30 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J15" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="K15" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="10:10">
-      <c r="J16" s="17" t="s">
+      <c r="J16" s="16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2598,31 +2600,31 @@
       <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>21</v>
       </c>
       <c r="G17" t="s">
         <v>1</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="17" t="s">
         <v>22</v>
       </c>
       <c r="J17" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="18" t="s">
+      <c r="K17" s="17" t="s">
         <v>24</v>
       </c>
       <c r="L17" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="18" t="s">
+      <c r="M17" s="17" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2630,31 +2632,31 @@
       <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J18" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="18" t="s">
+      <c r="K18" s="17" t="s">
         <v>26</v>
       </c>
       <c r="L18" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="18" t="s">
+      <c r="M18" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2662,31 +2664,31 @@
       <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="17" t="s">
         <v>21</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="17" t="s">
         <v>22</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="K19" s="17" t="s">
         <v>28</v>
       </c>
       <c r="L19" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="18" t="s">
+      <c r="M19" s="17" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2694,31 +2696,31 @@
       <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
         <v>9</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J20" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="18" t="s">
+      <c r="K20" s="17" t="s">
         <v>30</v>
       </c>
       <c r="L20" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="18" t="s">
+      <c r="M20" s="17" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2726,13 +2728,13 @@
       <c r="J21" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="18" t="s">
+      <c r="K21" s="17" t="s">
         <v>32</v>
       </c>
       <c r="L21" t="s">
         <v>23</v>
       </c>
-      <c r="M21" s="18" t="s">
+      <c r="M21" s="17" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2740,31 +2742,31 @@
       <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="17" t="s">
         <v>35</v>
       </c>
       <c r="G22" t="s">
         <v>1</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="17" t="s">
         <v>36</v>
       </c>
       <c r="J22" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="18" t="s">
+      <c r="K22" s="17" t="s">
         <v>37</v>
       </c>
       <c r="L22" t="s">
         <v>23</v>
       </c>
-      <c r="M22" s="18" t="s">
+      <c r="M22" s="17" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2772,31 +2774,31 @@
       <c r="A23" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G23" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H23" s="17" t="s">
         <v>7</v>
       </c>
       <c r="J23" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="18" t="s">
+      <c r="K23" s="17" t="s">
         <v>39</v>
       </c>
       <c r="L23" t="s">
         <v>23</v>
       </c>
-      <c r="M23" s="18" t="s">
+      <c r="M23" s="17" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2804,31 +2806,31 @@
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="17" t="s">
         <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="17" t="s">
         <v>35</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="17" t="s">
         <v>36</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="18" t="s">
+      <c r="K24" s="17" t="s">
         <v>41</v>
       </c>
       <c r="L24" t="s">
         <v>23</v>
       </c>
-      <c r="M24" s="18" t="s">
+      <c r="M24" s="17" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2836,31 +2838,31 @@
       <c r="A25" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="17" t="s">
         <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="17" t="s">
         <v>10</v>
       </c>
       <c r="J25" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="18" t="s">
+      <c r="K25" s="17" t="s">
         <v>43</v>
       </c>
       <c r="L25" t="s">
         <v>23</v>
       </c>
-      <c r="M25" s="18" t="s">
+      <c r="M25" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2883,32 +2885,32 @@
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2933,257 +2935,257 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="13" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="13" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="13" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="13" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="13" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="13" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="13" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="13" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="13" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="13" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="13" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="13" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3198,8 +3200,8 @@
   <sheetPr/>
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -3210,7 +3212,7 @@
     <col min="6" max="6" width="15.1111111111111" customWidth="1"/>
     <col min="7" max="7" width="23.5555555555556" customWidth="1"/>
     <col min="8" max="8" width="20.4444444444444" customWidth="1"/>
-    <col min="9" max="9" width="13.8888888888889" customWidth="1"/>
+    <col min="9" max="9" width="22.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3247,10 +3249,10 @@
       <c r="A4" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>110</v>
       </c>
     </row>
@@ -3297,13 +3299,13 @@
       <c r="A9" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="17" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3325,13 +3327,13 @@
       <c r="A11" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>129</v>
       </c>
     </row>
@@ -3355,10 +3357,10 @@
       <c r="A15" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="17" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3410,10 +3412,10 @@
       <c r="A20" t="s">
         <v>142</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="17" t="s">
         <v>143</v>
       </c>
     </row>
@@ -3478,19 +3480,19 @@
       <c r="A25" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="17" t="s">
         <v>155</v>
       </c>
       <c r="D25" t="s">
         <v>156</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="17" t="s">
         <v>155</v>
       </c>
       <c r="I25" t="s">
@@ -3547,22 +3549,22 @@
       <c r="A28" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="G28" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="17" t="s">
         <v>162</v>
       </c>
     </row>
@@ -3602,19 +3604,19 @@
       <c r="A32" t="s">
         <v>169</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="17" t="s">
         <v>171</v>
       </c>
     </row>
@@ -3705,11 +3707,11 @@
     <row r="40" spans="1:1">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>102</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="17" t="s">
         <v>191</v>
       </c>
       <c r="C41" t="s">
@@ -3718,7 +3720,7 @@
       <c r="D41">
         <v>12345</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="17" t="s">
         <v>191</v>
       </c>
       <c r="F41" t="s">
@@ -3727,8 +3729,11 @@
       <c r="H41" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -3747,36 +3752,42 @@
       <c r="G42" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="H42" s="9" t="s">
+      <c r="H42" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>197</v>
       </c>
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="G43" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="20" t="s">
         <v>202</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -3784,69 +3795,69 @@
         <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C47" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C48" s="17" t="s">
         <v>206</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>120</v>
       </c>
-      <c r="B49" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="C49" s="18" t="s">
+      <c r="B49" s="17" t="s">
         <v>208</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>123</v>
       </c>
-      <c r="B50" s="18" t="s">
-        <v>209</v>
+      <c r="B50" s="17" t="s">
+        <v>210</v>
       </c>
       <c r="C50" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>126</v>
       </c>
-      <c r="B51" s="18" t="s">
-        <v>211</v>
+      <c r="B51" s="17" t="s">
+        <v>212</v>
       </c>
       <c r="C51" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D53" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="4:4">
-      <c r="D54" s="11"/>
+      <c r="D54" s="10"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
@@ -3856,24 +3867,24 @@
         <v>104</v>
       </c>
       <c r="C55" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D55" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>217</v>
-      </c>
-      <c r="B56" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="B56" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="C56" s="18" t="s">
-        <v>218</v>
+      <c r="C56" s="17" t="s">
+        <v>219</v>
       </c>
       <c r="D56" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -3881,13 +3892,13 @@
         <v>134</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C57" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D57" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -3895,69 +3906,69 @@
         <v>136</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D58" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>138</v>
       </c>
-      <c r="B59" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>226</v>
+      <c r="B59" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>140</v>
       </c>
-      <c r="B60" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>227</v>
+      <c r="B60" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>228</v>
-      </c>
-      <c r="B61" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="C61" s="18" t="s">
+      <c r="B61" s="18" t="s">
         <v>230</v>
       </c>
+      <c r="C61" s="17" t="s">
+        <v>231</v>
+      </c>
       <c r="D61" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>144</v>
       </c>
-      <c r="B62" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>232</v>
+      <c r="B62" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -3965,9 +3976,9 @@
         <v>134</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D64" s="11"/>
+        <v>215</v>
+      </c>
+      <c r="D64" s="10"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
@@ -3977,10 +3988,10 @@
         <v>151</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D66" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -3991,38 +4002,38 @@
         <v>157</v>
       </c>
       <c r="C67" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D67" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>138</v>
       </c>
-      <c r="B68" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="D68" s="12" t="s">
-        <v>226</v>
+      <c r="B68" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>237</v>
-      </c>
-      <c r="B69" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B69" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="C69" s="18" t="s">
-        <v>238</v>
+      <c r="C69" s="17" t="s">
+        <v>239</v>
       </c>
       <c r="D69" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -4033,10 +4044,10 @@
         <v>177</v>
       </c>
       <c r="C70" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D70" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="72" spans="1:1">
@@ -4046,24 +4057,24 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B74" t="s">
         <v>167</v>
       </c>
       <c r="C74" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>244</v>
-      </c>
-      <c r="B75" s="18" t="s">
         <v>245</v>
       </c>
+      <c r="B75" s="17" t="s">
+        <v>246</v>
+      </c>
       <c r="C75" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -4071,21 +4082,21 @@
         <v>173</v>
       </c>
       <c r="B76" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C76" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B77" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C77" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -4093,10 +4104,10 @@
         <v>179</v>
       </c>
       <c r="B78" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C78" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -4110,6 +4121,7 @@
     <hyperlink ref="G42" r:id="rId4" display="pavanikaka@gmail.com"/>
     <hyperlink ref="C58" r:id="rId5" display="Hyd@#"/>
     <hyperlink ref="H42" r:id="rId6" display="148@#$"/>
+    <hyperlink ref="I42" r:id="rId4" display="pavanikaka@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>